<commit_message>
Börjat på ett skript för analys av lyvariabler och städat lydatan. Har printat en fil med allt sammanställt. Dock är den kort. Ändrat lynamnen i tor.lydata.sommar och tor.lydata. Lagt till standardisering med partial standard deviations till AIC-analys av kärnlyor Helags. Dessutom har jag ändrat kvadratmeter till kvadratkm och meter till km för variablerna i dens.sub-dataramen. Detta för att kunna lägga på en linjär modell på datat för att få ut partial standard deviations. Därefter gör man en ny linjär modell där man tar med partial standard deviations.
</commit_message>
<xml_diff>
--- a/Rawdata/tor.lydata.sommar.xlsx
+++ b/Rawdata/tor.lydata.sommar.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torhanssonfrank/Desktop/Skolarbeten/Master i Stockholm/Masterarbete/Den and territory selection/Rawdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37649CD-D679-DD4B-BB60-09DEA8BA7495}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="13800" xr2:uid="{BD9596F3-B6C2-EC43-92CA-E0BA01C042D5}"/>
+    <workbookView xWindow="2280" yWindow="1060" windowWidth="28340" windowHeight="13800" xr2:uid="{BD9596F3-B6C2-EC43-92CA-E0BA01C042D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="37">
-  <si>
-    <t>lya</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="36">
   <si>
     <t>lufttemp</t>
   </si>
@@ -59,9 +57,6 @@
     <t>area</t>
   </si>
   <si>
-    <t>zz104</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -74,55 +69,16 @@
     <t>j</t>
   </si>
   <si>
-    <t>zz042</t>
-  </si>
-  <si>
-    <t>zz042b</t>
-  </si>
-  <si>
-    <t>zz042 har en liten "bonuslya" som ligger c:a 150 meter från huvudlyan. Frågan är om den ska med i analysen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lyan har lite olika riktningar. Den branta delens riktning är 22° med lutning(vinkel) 34°. Den delen har dock en mindre platt del under sig. Den branta delen plus den lilla platta delen har tillsammans vinkel 17° (antagligen den vettigaste vinkeln att använda).  Den stora platta delen på lyans topp har riktning 116° och lutning 3°. </t>
-  </si>
-  <si>
-    <t>zz020</t>
-  </si>
-  <si>
     <t>Även den här lyan har en liten filial men den ligger i anslutning till lyan. Dess lyöppningar (13) och area är inräknat i totalen.</t>
-  </si>
-  <si>
-    <t>zz033</t>
   </si>
   <si>
     <t>rendelar, fjädrar, sork och lämmel på lyan. Såg ingen räv.</t>
   </si>
   <si>
-    <t>zz099</t>
-  </si>
-  <si>
-    <t>zz062</t>
-  </si>
-  <si>
-    <t>zz096</t>
-  </si>
-  <si>
-    <t>zz014</t>
-  </si>
-  <si>
-    <t>zz061</t>
-  </si>
-  <si>
     <t>lyan har nog varit större innan men svårt att säga hur stor</t>
   </si>
   <si>
-    <t>zz075</t>
-  </si>
-  <si>
     <t>platt lya, svårt att bestämma riktning</t>
-  </si>
-  <si>
-    <t>zz076</t>
   </si>
   <si>
     <t>grävt lite halvhjärtat i ett hål men definitivt inte aktiv</t>
@@ -136,18 +92,67 @@
   <si>
     <t>den mindre lydelen har riktning 64° och vinkel 17°. Lydelarna sitter ihop. Arean är för hela lyan</t>
   </si>
+  <si>
+    <t>Namn</t>
+  </si>
+  <si>
+    <t>fszz104</t>
+  </si>
+  <si>
+    <t>fszz042</t>
+  </si>
+  <si>
+    <t>fszz020</t>
+  </si>
+  <si>
+    <t>fszz033</t>
+  </si>
+  <si>
+    <t>fszz099</t>
+  </si>
+  <si>
+    <t>fszz062</t>
+  </si>
+  <si>
+    <t>fszz096</t>
+  </si>
+  <si>
+    <t>fszz014</t>
+  </si>
+  <si>
+    <t>fszz061</t>
+  </si>
+  <si>
+    <t>fszz075</t>
+  </si>
+  <si>
+    <t>fszz076</t>
+  </si>
+  <si>
+    <t>1338.9927</t>
+  </si>
+  <si>
+    <t>Lyan har lite olika riktningar. Den branta delens riktning är 22° med lutning(vinkel) 34°. Den delen har dock en mindre platt del under sig. Den branta delen plus den lilla platta delen har tillsammans vinkel 17° (antagligen den vettigaste vinkeln att använda).  Den stora platta delen på lyans topp har riktning 116° och lutning 3°. La till filialens area och lyöppningar (8) i totalen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF101010"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,8 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,53 +494,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2A87BE-6D2E-1146-8DC2-BF63A48815A4}">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
+    </row>
+    <row r="2" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
         <v>125.58374999999999</v>
@@ -544,7 +556,7 @@
         <v>8.5</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>80</v>
@@ -556,15 +568,16 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B3">
         <v>125.58374999999999</v>
@@ -576,7 +589,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>80</v>
@@ -588,15 +601,15 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B4">
         <v>125.58374999999999</v>
@@ -608,7 +621,7 @@
         <v>7.9</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>80</v>
@@ -620,15 +633,15 @@
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B5">
         <v>125.58374999999999</v>
@@ -640,7 +653,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>80</v>
@@ -652,15 +665,15 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B6">
         <v>125.58374999999999</v>
@@ -672,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>80</v>
@@ -684,15 +697,15 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B7">
         <v>125.58374999999999</v>
@@ -704,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>80</v>
@@ -716,15 +729,15 @@
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B8">
         <v>125.58374999999999</v>
@@ -736,7 +749,7 @@
         <v>6.1</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>80</v>
@@ -748,15 +761,15 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B9">
         <v>125.58374999999999</v>
@@ -768,7 +781,7 @@
         <v>6.6</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>80</v>
@@ -780,15 +793,15 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B10">
         <v>125.58374999999999</v>
@@ -800,7 +813,7 @@
         <v>7.5</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>80</v>
@@ -812,15 +825,15 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B11">
         <v>125.58374999999999</v>
@@ -832,7 +845,7 @@
         <v>6.2</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>80</v>
@@ -844,18 +857,18 @@
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>1208.3856000000001</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
       <c r="C12">
         <v>6.3</v>
@@ -864,30 +877,30 @@
         <v>6.5</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>22</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I12">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>1208.3856000000001</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
       </c>
       <c r="C13">
         <v>6.3</v>
@@ -896,30 +909,30 @@
         <v>7.3</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>22</v>
       </c>
       <c r="H13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I13">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>1208.3856000000001</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
       </c>
       <c r="C14">
         <v>6.3</v>
@@ -928,30 +941,30 @@
         <v>6.8</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>22</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I14">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>1208.3856000000001</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
       </c>
       <c r="C15">
         <v>6.3</v>
@@ -960,30 +973,30 @@
         <v>6.8</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15">
         <v>22</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I15">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>1208.3856000000001</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
       </c>
       <c r="C16">
         <v>6.3</v>
@@ -992,30 +1005,30 @@
         <v>6.7</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>22</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I16">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1208.3856000000001</v>
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
       </c>
       <c r="C17">
         <v>6.3</v>
@@ -1024,30 +1037,30 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <v>22</v>
       </c>
       <c r="H17">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I17">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>1208.3856000000001</v>
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
       </c>
       <c r="C18">
         <v>6.3</v>
@@ -1056,30 +1069,30 @@
         <v>7.8</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18">
         <v>22</v>
       </c>
       <c r="H18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I18">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>1208.3856000000001</v>
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
       <c r="C19">
         <v>6.3</v>
@@ -1088,30 +1101,30 @@
         <v>7.3</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19">
         <v>22</v>
       </c>
       <c r="H19">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I19">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>1208.3856000000001</v>
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
       </c>
       <c r="C20">
         <v>6.3</v>
@@ -1120,30 +1133,30 @@
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <v>22</v>
       </c>
       <c r="H20">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>1208.3856000000001</v>
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
       </c>
       <c r="C21">
         <v>6.3</v>
@@ -1152,44 +1165,59 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <v>22</v>
       </c>
       <c r="H21">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I21">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>17</v>
+      <c r="A22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>130.6071</v>
+        <v>1230.5125</v>
+      </c>
+      <c r="C22">
+        <v>5.5</v>
+      </c>
+      <c r="D22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>88</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
       </c>
       <c r="I22">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>20</v>
+      <c r="A23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1230.5125</v>
@@ -1198,10 +1226,10 @@
         <v>5.5</v>
       </c>
       <c r="D23">
-        <v>2.2999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G23">
         <v>88</v>
@@ -1213,15 +1241,15 @@
         <v>90</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>20</v>
+      <c r="A24" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B24">
         <v>1230.5125</v>
@@ -1230,10 +1258,10 @@
         <v>5.5</v>
       </c>
       <c r="D24">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G24">
         <v>88</v>
@@ -1245,15 +1273,15 @@
         <v>90</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>20</v>
+      <c r="A25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B25">
         <v>1230.5125</v>
@@ -1262,10 +1290,10 @@
         <v>5.5</v>
       </c>
       <c r="D25">
-        <v>5.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G25">
         <v>88</v>
@@ -1277,15 +1305,15 @@
         <v>90</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K25" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>20</v>
+      <c r="A26" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B26">
         <v>1230.5125</v>
@@ -1294,10 +1322,10 @@
         <v>5.5</v>
       </c>
       <c r="D26">
-        <v>2.2999999999999998</v>
+        <v>4.2</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26">
         <v>88</v>
@@ -1309,15 +1337,15 @@
         <v>90</v>
       </c>
       <c r="J26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K26" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>20</v>
+      <c r="A27" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B27">
         <v>1230.5125</v>
@@ -1326,10 +1354,10 @@
         <v>5.5</v>
       </c>
       <c r="D27">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G27">
         <v>88</v>
@@ -1341,15 +1369,15 @@
         <v>90</v>
       </c>
       <c r="J27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>20</v>
+      <c r="A28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B28">
         <v>1230.5125</v>
@@ -1358,10 +1386,10 @@
         <v>5.5</v>
       </c>
       <c r="D28">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G28">
         <v>88</v>
@@ -1373,15 +1401,15 @@
         <v>90</v>
       </c>
       <c r="J28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>20</v>
+      <c r="A29" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B29">
         <v>1230.5125</v>
@@ -1390,10 +1418,10 @@
         <v>5.5</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29">
         <v>88</v>
@@ -1405,15 +1433,15 @@
         <v>90</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K29" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>20</v>
+      <c r="A30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B30">
         <v>1230.5125</v>
@@ -1422,10 +1450,10 @@
         <v>5.5</v>
       </c>
       <c r="D30">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G30">
         <v>88</v>
@@ -1437,15 +1465,15 @@
         <v>90</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>20</v>
+      <c r="A31" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B31">
         <v>1230.5125</v>
@@ -1454,10 +1482,10 @@
         <v>5.5</v>
       </c>
       <c r="D31">
-        <v>3.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G31">
         <v>88</v>
@@ -1469,47 +1497,50 @@
         <v>90</v>
       </c>
       <c r="J31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>420.17500000000001</v>
+      </c>
+      <c r="C32">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D32">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>8.9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>212</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <v>35</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
         <v>15</v>
       </c>
-      <c r="K31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32">
-        <v>1230.5125</v>
-      </c>
-      <c r="C32">
-        <v>5.5</v>
-      </c>
-      <c r="D32">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32">
-        <v>88</v>
-      </c>
-      <c r="H32">
-        <v>9</v>
-      </c>
-      <c r="I32">
-        <v>90</v>
-      </c>
-      <c r="J32" t="s">
-        <v>15</v>
-      </c>
-      <c r="K32" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>22</v>
+      <c r="A33" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B33">
         <v>420.17500000000001</v>
@@ -1518,13 +1549,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D33">
-        <v>9</v>
+        <v>7.6</v>
       </c>
       <c r="E33">
-        <v>8.9</v>
+        <v>7.9</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G33">
         <v>212</v>
@@ -1536,15 +1567,15 @@
         <v>35</v>
       </c>
       <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" t="s">
         <v>15</v>
       </c>
-      <c r="K33" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>22</v>
+      <c r="A34" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B34">
         <v>420.17500000000001</v>
@@ -1553,13 +1584,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D34">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
       <c r="E34">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34">
         <v>212</v>
@@ -1571,15 +1602,15 @@
         <v>35</v>
       </c>
       <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" t="s">
         <v>15</v>
       </c>
-      <c r="K34" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>22</v>
+      <c r="A35" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B35">
         <v>420.17500000000001</v>
@@ -1588,13 +1619,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D35">
-        <v>7.8</v>
+        <v>8.5</v>
       </c>
       <c r="E35">
-        <v>8.1</v>
+        <v>8.4</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35">
         <v>212</v>
@@ -1606,15 +1637,15 @@
         <v>35</v>
       </c>
       <c r="J35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" t="s">
         <v>15</v>
       </c>
-      <c r="K35" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>22</v>
+      <c r="A36" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B36">
         <v>420.17500000000001</v>
@@ -1623,13 +1654,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D36">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
       <c r="E36">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>212</v>
@@ -1641,15 +1672,15 @@
         <v>35</v>
       </c>
       <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" t="s">
         <v>15</v>
       </c>
-      <c r="K36" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>22</v>
+      <c r="A37" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B37">
         <v>420.17500000000001</v>
@@ -1661,10 +1692,10 @@
         <v>7.6</v>
       </c>
       <c r="E37">
-        <v>8.1</v>
+        <v>7.4</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37">
         <v>212</v>
@@ -1676,15 +1707,15 @@
         <v>35</v>
       </c>
       <c r="J37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" t="s">
         <v>15</v>
       </c>
-      <c r="K37" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>22</v>
+      <c r="A38" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B38">
         <v>420.17500000000001</v>
@@ -1693,13 +1724,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D38">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
       <c r="E38">
-        <v>7.4</v>
+        <v>7.1</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G38">
         <v>212</v>
@@ -1711,15 +1742,15 @@
         <v>35</v>
       </c>
       <c r="J38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" t="s">
         <v>15</v>
       </c>
-      <c r="K38" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>22</v>
+      <c r="A39" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B39">
         <v>420.17500000000001</v>
@@ -1728,13 +1759,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D39">
-        <v>7.8</v>
+        <v>6.5</v>
       </c>
       <c r="E39">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G39">
         <v>212</v>
@@ -1746,15 +1777,15 @@
         <v>35</v>
       </c>
       <c r="J39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" t="s">
         <v>15</v>
       </c>
-      <c r="K39" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>22</v>
+      <c r="A40" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B40">
         <v>420.17500000000001</v>
@@ -1763,13 +1794,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D40">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="E40">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G40">
         <v>212</v>
@@ -1781,15 +1812,15 @@
         <v>35</v>
       </c>
       <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
         <v>15</v>
       </c>
-      <c r="K40" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>22</v>
+      <c r="A41" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B41">
         <v>420.17500000000001</v>
@@ -1798,13 +1829,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="E41">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G41">
         <v>212</v>
@@ -1816,50 +1847,47 @@
         <v>35</v>
       </c>
       <c r="J41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" t="s">
         <v>15</v>
       </c>
-      <c r="K41" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>22</v>
+      <c r="A42" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B42">
-        <v>420.17500000000001</v>
+        <v>150.0625</v>
       </c>
       <c r="C42">
         <v>8.6999999999999993</v>
       </c>
       <c r="D42">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="E42">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G42">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="H42">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I42">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>15</v>
-      </c>
-      <c r="K42" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>24</v>
+      <c r="A43" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B43">
         <v>150.0625</v>
@@ -1868,13 +1896,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D43">
-        <v>7.2</v>
+        <v>7.5</v>
       </c>
       <c r="E43">
-        <v>7</v>
+        <v>7.9</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G43">
         <v>236</v>
@@ -1886,12 +1914,12 @@
         <v>8</v>
       </c>
       <c r="J43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>24</v>
+      <c r="A44" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B44">
         <v>150.0625</v>
@@ -1900,13 +1928,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D44">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="E44">
-        <v>7.9</v>
+        <v>7.2</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>236</v>
@@ -1918,12 +1946,12 @@
         <v>8</v>
       </c>
       <c r="J44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>24</v>
+      <c r="A45" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B45">
         <v>150.0625</v>
@@ -1932,13 +1960,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D45">
-        <v>7.3</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E45">
-        <v>7.2</v>
+        <v>9.1</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <v>236</v>
@@ -1950,12 +1978,12 @@
         <v>8</v>
       </c>
       <c r="J45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>24</v>
+      <c r="A46" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B46">
         <v>150.0625</v>
@@ -1964,13 +1992,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D46">
-        <v>9.1999999999999993</v>
+        <v>7.2</v>
       </c>
       <c r="E46">
-        <v>9.1</v>
+        <v>7.3</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G46">
         <v>236</v>
@@ -1982,12 +2010,12 @@
         <v>8</v>
       </c>
       <c r="J46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>24</v>
+      <c r="A47" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B47">
         <v>150.0625</v>
@@ -1996,13 +2024,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D47">
-        <v>7.2</v>
+        <v>8.6</v>
       </c>
       <c r="E47">
-        <v>7.3</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G47">
         <v>236</v>
@@ -2014,12 +2042,12 @@
         <v>8</v>
       </c>
       <c r="J47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>24</v>
+      <c r="A48" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B48">
         <v>150.0625</v>
@@ -2028,13 +2056,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D48">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="E48">
-        <v>8.8000000000000007</v>
+        <v>7.9</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G48">
         <v>236</v>
@@ -2046,12 +2074,12 @@
         <v>8</v>
       </c>
       <c r="J48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>24</v>
+      <c r="A49" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B49">
         <v>150.0625</v>
@@ -2060,13 +2088,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D49">
-        <v>8.9</v>
+        <v>8.4</v>
       </c>
       <c r="E49">
-        <v>7.9</v>
+        <v>8.6</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49">
         <v>236</v>
@@ -2078,12 +2106,12 @@
         <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>24</v>
+      <c r="A50" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B50">
         <v>150.0625</v>
@@ -2092,13 +2120,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D50">
-        <v>8.4</v>
+        <v>6.5</v>
       </c>
       <c r="E50">
-        <v>8.6</v>
+        <v>6.8</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G50">
         <v>236</v>
@@ -2110,12 +2138,12 @@
         <v>8</v>
       </c>
       <c r="J50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>24</v>
+      <c r="A51" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B51">
         <v>150.0625</v>
@@ -2124,13 +2152,13 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D51">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G51">
         <v>236</v>
@@ -2142,44 +2170,47 @@
         <v>8</v>
       </c>
       <c r="J51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>24</v>
+      <c r="A52" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B52">
-        <v>150.0625</v>
+        <v>195.08125000000001</v>
       </c>
       <c r="C52">
-        <v>8.6999999999999993</v>
+        <v>18</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>12.9</v>
       </c>
       <c r="E52">
-        <v>6.7</v>
+        <v>11.8</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G52">
         <v>236</v>
       </c>
       <c r="H52">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I52">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J52" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="K52" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>25</v>
+      <c r="A53" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B53">
         <v>195.08125000000001</v>
@@ -2188,13 +2219,13 @@
         <v>18</v>
       </c>
       <c r="D53">
-        <v>12.9</v>
+        <v>11.2</v>
       </c>
       <c r="E53">
-        <v>11.8</v>
+        <v>12.5</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G53">
         <v>236</v>
@@ -2206,15 +2237,15 @@
         <v>25</v>
       </c>
       <c r="J53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K53" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>25</v>
+      <c r="A54" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B54">
         <v>195.08125000000001</v>
@@ -2223,13 +2254,13 @@
         <v>18</v>
       </c>
       <c r="D54">
-        <v>11.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E54">
-        <v>12.5</v>
+        <v>8.5</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G54">
         <v>236</v>
@@ -2241,15 +2272,15 @@
         <v>25</v>
       </c>
       <c r="J54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K54" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>25</v>
+      <c r="A55" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B55">
         <v>195.08125000000001</v>
@@ -2258,13 +2289,13 @@
         <v>18</v>
       </c>
       <c r="D55">
-        <v>8.1999999999999993</v>
+        <v>8.5</v>
       </c>
       <c r="E55">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G55">
         <v>236</v>
@@ -2276,15 +2307,15 @@
         <v>25</v>
       </c>
       <c r="J55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K55" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>25</v>
+      <c r="A56" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B56">
         <v>195.08125000000001</v>
@@ -2293,13 +2324,13 @@
         <v>18</v>
       </c>
       <c r="D56">
-        <v>8.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E56">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G56">
         <v>236</v>
@@ -2311,15 +2342,15 @@
         <v>25</v>
       </c>
       <c r="J56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K56" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>25</v>
+      <c r="A57" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B57">
         <v>195.08125000000001</v>
@@ -2328,13 +2359,13 @@
         <v>18</v>
       </c>
       <c r="D57">
-        <v>8.3000000000000007</v>
+        <v>9.1</v>
       </c>
       <c r="E57">
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G57">
         <v>236</v>
@@ -2346,15 +2377,15 @@
         <v>25</v>
       </c>
       <c r="J57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K57" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>25</v>
+      <c r="A58" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B58">
         <v>195.08125000000001</v>
@@ -2363,13 +2394,13 @@
         <v>18</v>
       </c>
       <c r="D58">
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="E58">
-        <v>8.6</v>
+        <v>8.4</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G58">
         <v>236</v>
@@ -2381,15 +2412,15 @@
         <v>25</v>
       </c>
       <c r="J58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K58" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>25</v>
+      <c r="A59" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B59">
         <v>195.08125000000001</v>
@@ -2398,13 +2429,13 @@
         <v>18</v>
       </c>
       <c r="D59">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="E59">
-        <v>8.4</v>
+        <v>7.1</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G59">
         <v>236</v>
@@ -2416,15 +2447,15 @@
         <v>25</v>
       </c>
       <c r="J59" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K59" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>25</v>
+      <c r="A60" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B60">
         <v>195.08125000000001</v>
@@ -2433,13 +2464,13 @@
         <v>18</v>
       </c>
       <c r="D60">
-        <v>7.1</v>
+        <v>8.6</v>
       </c>
       <c r="E60">
-        <v>7.1</v>
+        <v>8.9</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G60">
         <v>236</v>
@@ -2451,15 +2482,15 @@
         <v>25</v>
       </c>
       <c r="J60" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K60" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>25</v>
+      <c r="A61" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B61">
         <v>195.08125000000001</v>
@@ -2468,13 +2499,13 @@
         <v>18</v>
       </c>
       <c r="D61">
-        <v>8.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E61">
-        <v>8.9</v>
+        <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G61">
         <v>236</v>
@@ -2486,50 +2517,50 @@
         <v>25</v>
       </c>
       <c r="J61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K61" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>25</v>
+      <c r="A62" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B62">
-        <v>195.08125000000001</v>
+        <v>84.034999999999997</v>
       </c>
       <c r="C62">
-        <v>18</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="D62">
-        <v>9.3000000000000007</v>
+        <v>7.2</v>
       </c>
       <c r="E62">
-        <v>9</v>
+        <v>7.3</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G62">
-        <v>236</v>
+        <v>288</v>
       </c>
       <c r="H62">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I62">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>26</v>
+      <c r="A63" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B63">
         <v>84.034999999999997</v>
@@ -2538,13 +2569,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D63">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="E63">
         <v>7.3</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G63">
         <v>288</v>
@@ -2556,15 +2587,15 @@
         <v>11</v>
       </c>
       <c r="J63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K63" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>26</v>
+      <c r="A64" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B64">
         <v>84.034999999999997</v>
@@ -2579,7 +2610,7 @@
         <v>7.3</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G64">
         <v>288</v>
@@ -2591,15 +2622,15 @@
         <v>11</v>
       </c>
       <c r="J64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K64" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>26</v>
+      <c r="A65" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B65">
         <v>84.034999999999997</v>
@@ -2608,13 +2639,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D65">
-        <v>7.3</v>
+        <v>8</v>
       </c>
       <c r="E65">
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G65">
         <v>288</v>
@@ -2626,15 +2657,15 @@
         <v>11</v>
       </c>
       <c r="J65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K65" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>26</v>
+      <c r="A66" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B66">
         <v>84.034999999999997</v>
@@ -2643,13 +2674,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D66">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E66">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="F66" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G66">
         <v>288</v>
@@ -2661,15 +2692,15 @@
         <v>11</v>
       </c>
       <c r="J66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K66" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>26</v>
+      <c r="A67" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B67">
         <v>84.034999999999997</v>
@@ -2678,13 +2709,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D67">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="E67">
-        <v>7.6</v>
+        <v>7.4</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G67">
         <v>288</v>
@@ -2696,15 +2727,15 @@
         <v>11</v>
       </c>
       <c r="J67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K67" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>26</v>
+      <c r="A68" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B68">
         <v>84.034999999999997</v>
@@ -2713,13 +2744,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D68">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="E68">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G68">
         <v>288</v>
@@ -2731,15 +2762,15 @@
         <v>11</v>
       </c>
       <c r="J68" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K68" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>26</v>
+      <c r="A69" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B69">
         <v>84.034999999999997</v>
@@ -2748,13 +2779,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D69">
-        <v>7.2</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E69">
-        <v>7.3</v>
+        <v>8.4</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G69">
         <v>288</v>
@@ -2766,15 +2797,15 @@
         <v>11</v>
       </c>
       <c r="J69" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K69" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>26</v>
+      <c r="A70" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B70">
         <v>84.034999999999997</v>
@@ -2786,10 +2817,10 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="E70">
-        <v>8.4</v>
+        <v>8.9</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G70">
         <v>288</v>
@@ -2801,15 +2832,15 @@
         <v>11</v>
       </c>
       <c r="J70" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K70" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>26</v>
+      <c r="A71" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B71">
         <v>84.034999999999997</v>
@@ -2818,13 +2849,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D71">
-        <v>8.8000000000000007</v>
+        <v>10.4</v>
       </c>
       <c r="E71">
-        <v>8.9</v>
+        <v>10.5</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G71">
         <v>288</v>
@@ -2836,50 +2867,50 @@
         <v>11</v>
       </c>
       <c r="J71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K71" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>26</v>
+      <c r="A72" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B72">
-        <v>84.034999999999997</v>
+        <v>909.41399999999999</v>
       </c>
       <c r="C72">
-        <v>20.100000000000001</v>
+        <v>12.3</v>
       </c>
       <c r="D72">
-        <v>10.4</v>
+        <v>7.7</v>
       </c>
       <c r="E72">
-        <v>10.5</v>
+        <v>7.6</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G72">
-        <v>288</v>
+        <v>124</v>
       </c>
       <c r="H72">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="I72">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="J72" t="s">
         <v>13</v>
       </c>
       <c r="K72" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>27</v>
+      <c r="A73" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B73">
         <v>909.41399999999999</v>
@@ -2888,13 +2919,13 @@
         <v>12.3</v>
       </c>
       <c r="D73">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E73">
-        <v>7.6</v>
+        <v>8.6</v>
       </c>
       <c r="F73" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G73">
         <v>124</v>
@@ -2906,15 +2937,15 @@
         <v>70</v>
       </c>
       <c r="J73" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K73" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>27</v>
+      <c r="A74" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B74">
         <v>909.41399999999999</v>
@@ -2923,13 +2954,13 @@
         <v>12.3</v>
       </c>
       <c r="D74">
-        <v>8.6999999999999993</v>
+        <v>7.7</v>
       </c>
       <c r="E74">
-        <v>8.6</v>
+        <v>7.3</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G74">
         <v>124</v>
@@ -2941,15 +2972,15 @@
         <v>70</v>
       </c>
       <c r="J74" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K74" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>27</v>
+      <c r="A75" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B75">
         <v>909.41399999999999</v>
@@ -2958,13 +2989,13 @@
         <v>12.3</v>
       </c>
       <c r="D75">
-        <v>7.7</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E75">
-        <v>7.3</v>
+        <v>8.1</v>
       </c>
       <c r="F75" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G75">
         <v>124</v>
@@ -2976,15 +3007,15 @@
         <v>70</v>
       </c>
       <c r="J75" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K75" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>27</v>
+      <c r="A76" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B76">
         <v>909.41399999999999</v>
@@ -2993,13 +3024,13 @@
         <v>12.3</v>
       </c>
       <c r="D76">
-        <v>8.1999999999999993</v>
+        <v>10.1</v>
       </c>
       <c r="E76">
-        <v>8.1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G76">
         <v>124</v>
@@ -3011,15 +3042,15 @@
         <v>70</v>
       </c>
       <c r="J76" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K76" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>27</v>
+      <c r="A77" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B77">
         <v>909.41399999999999</v>
@@ -3028,13 +3059,13 @@
         <v>12.3</v>
       </c>
       <c r="D77">
-        <v>10.1</v>
+        <v>9</v>
       </c>
       <c r="E77">
-        <v>10</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G77">
         <v>124</v>
@@ -3046,15 +3077,15 @@
         <v>70</v>
       </c>
       <c r="J77" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K77" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>27</v>
+      <c r="A78" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B78">
         <v>909.41399999999999</v>
@@ -3063,13 +3094,13 @@
         <v>12.3</v>
       </c>
       <c r="D78">
-        <v>9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E78">
-        <v>8.6999999999999993</v>
+        <v>7.8</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G78">
         <v>124</v>
@@ -3081,15 +3112,15 @@
         <v>70</v>
       </c>
       <c r="J78" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K78" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>27</v>
+      <c r="A79" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B79">
         <v>909.41399999999999</v>
@@ -3098,13 +3129,13 @@
         <v>12.3</v>
       </c>
       <c r="D79">
-        <v>8.1999999999999993</v>
+        <v>8.5</v>
       </c>
       <c r="E79">
-        <v>7.8</v>
+        <v>8.5</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G79">
         <v>124</v>
@@ -3116,15 +3147,15 @@
         <v>70</v>
       </c>
       <c r="J79" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K79" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>27</v>
+      <c r="A80" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B80">
         <v>909.41399999999999</v>
@@ -3133,13 +3164,13 @@
         <v>12.3</v>
       </c>
       <c r="D80">
-        <v>8.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E80">
-        <v>8.5</v>
+        <v>8.1</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G80">
         <v>124</v>
@@ -3151,50 +3182,50 @@
         <v>70</v>
       </c>
       <c r="J80" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K80" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>27</v>
+      <c r="A81" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B81">
-        <v>909.41399999999999</v>
+        <v>256.606875</v>
       </c>
       <c r="C81">
-        <v>12.3</v>
+        <v>21.4</v>
       </c>
       <c r="D81">
-        <v>8.1999999999999993</v>
+        <v>11.1</v>
       </c>
       <c r="E81">
-        <v>8.1</v>
+        <v>11.9</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G81">
-        <v>124</v>
+        <v>286</v>
       </c>
       <c r="H81">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I81">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="J81" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K81" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>28</v>
+      <c r="A82" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B82">
         <v>256.606875</v>
@@ -3203,13 +3234,13 @@
         <v>21.4</v>
       </c>
       <c r="D82">
-        <v>11.1</v>
+        <v>15.2</v>
       </c>
       <c r="E82">
-        <v>11.9</v>
+        <v>15.7</v>
       </c>
       <c r="F82" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G82">
         <v>286</v>
@@ -3221,15 +3252,15 @@
         <v>5</v>
       </c>
       <c r="J82" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K82" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>28</v>
+      <c r="A83" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B83">
         <v>256.606875</v>
@@ -3238,13 +3269,13 @@
         <v>21.4</v>
       </c>
       <c r="D83">
-        <v>15.2</v>
+        <v>11.3</v>
       </c>
       <c r="E83">
-        <v>15.7</v>
+        <v>10.9</v>
       </c>
       <c r="F83" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G83">
         <v>286</v>
@@ -3256,15 +3287,15 @@
         <v>5</v>
       </c>
       <c r="J83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K83" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>28</v>
+      <c r="A84" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B84">
         <v>256.606875</v>
@@ -3273,13 +3304,13 @@
         <v>21.4</v>
       </c>
       <c r="D84">
-        <v>11.3</v>
+        <v>12</v>
       </c>
       <c r="E84">
-        <v>10.9</v>
+        <v>11.6</v>
       </c>
       <c r="F84" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G84">
         <v>286</v>
@@ -3291,15 +3322,15 @@
         <v>5</v>
       </c>
       <c r="J84" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K84" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>28</v>
+      <c r="A85" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B85">
         <v>256.606875</v>
@@ -3308,13 +3339,13 @@
         <v>21.4</v>
       </c>
       <c r="D85">
-        <v>12</v>
+        <v>9.9</v>
       </c>
       <c r="E85">
-        <v>11.6</v>
+        <v>9.5</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G85">
         <v>286</v>
@@ -3326,15 +3357,15 @@
         <v>5</v>
       </c>
       <c r="J85" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K85" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>28</v>
+      <c r="A86" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B86">
         <v>256.606875</v>
@@ -3343,13 +3374,13 @@
         <v>21.4</v>
       </c>
       <c r="D86">
-        <v>9.9</v>
+        <v>13.7</v>
       </c>
       <c r="E86">
-        <v>9.5</v>
+        <v>13.4</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G86">
         <v>286</v>
@@ -3361,15 +3392,15 @@
         <v>5</v>
       </c>
       <c r="J86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K86" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>28</v>
+      <c r="A87" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B87">
         <v>256.606875</v>
@@ -3378,13 +3409,13 @@
         <v>21.4</v>
       </c>
       <c r="D87">
-        <v>13.7</v>
+        <v>9</v>
       </c>
       <c r="E87">
-        <v>13.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F87" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G87">
         <v>286</v>
@@ -3396,15 +3427,15 @@
         <v>5</v>
       </c>
       <c r="J87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K87" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>28</v>
+      <c r="A88" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B88">
         <v>256.606875</v>
@@ -3413,13 +3444,13 @@
         <v>21.4</v>
       </c>
       <c r="D88">
-        <v>9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E88">
-        <v>9.1999999999999993</v>
+        <v>7.4</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G88">
         <v>286</v>
@@ -3431,15 +3462,15 @@
         <v>5</v>
       </c>
       <c r="J88" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K88" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>28</v>
+      <c r="A89" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B89">
         <v>256.606875</v>
@@ -3448,13 +3479,13 @@
         <v>21.4</v>
       </c>
       <c r="D89">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="E89">
-        <v>7.4</v>
+        <v>7.7</v>
       </c>
       <c r="F89" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G89">
         <v>286</v>
@@ -3466,15 +3497,15 @@
         <v>5</v>
       </c>
       <c r="J89" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K89" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>28</v>
+      <c r="A90" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B90">
         <v>256.606875</v>
@@ -3483,13 +3514,13 @@
         <v>21.4</v>
       </c>
       <c r="D90">
-        <v>8.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E90">
-        <v>7.7</v>
+        <v>9.5</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G90">
         <v>286</v>
@@ -3501,50 +3532,50 @@
         <v>5</v>
       </c>
       <c r="J90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K90" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>28</v>
+      <c r="A91" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B91">
-        <v>256.606875</v>
+        <v>231.09625</v>
       </c>
       <c r="C91">
-        <v>21.4</v>
+        <v>8.4</v>
       </c>
       <c r="D91">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="E91">
-        <v>9.5</v>
+        <v>8.9</v>
       </c>
       <c r="F91" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G91">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="H91">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I91">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J91" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K91" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>30</v>
+      <c r="A92" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B92">
         <v>231.09625</v>
@@ -3553,13 +3584,13 @@
         <v>8.4</v>
       </c>
       <c r="D92">
-        <v>9.1</v>
+        <v>11</v>
       </c>
       <c r="E92">
-        <v>8.9</v>
+        <v>10.8</v>
       </c>
       <c r="F92" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G92">
         <v>248</v>
@@ -3571,15 +3602,15 @@
         <v>8</v>
       </c>
       <c r="J92" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>30</v>
+      <c r="A93" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B93">
         <v>231.09625</v>
@@ -3588,13 +3619,13 @@
         <v>8.4</v>
       </c>
       <c r="D93">
-        <v>11</v>
+        <v>8.5</v>
       </c>
       <c r="E93">
-        <v>10.8</v>
+        <v>8.4</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G93">
         <v>248</v>
@@ -3606,15 +3637,15 @@
         <v>8</v>
       </c>
       <c r="J93" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>30</v>
+      <c r="A94" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B94">
         <v>231.09625</v>
@@ -3623,13 +3654,13 @@
         <v>8.4</v>
       </c>
       <c r="D94">
-        <v>8.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E94">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G94">
         <v>248</v>
@@ -3641,15 +3672,15 @@
         <v>8</v>
       </c>
       <c r="J94" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>30</v>
+      <c r="A95" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B95">
         <v>231.09625</v>
@@ -3658,13 +3689,13 @@
         <v>8.4</v>
       </c>
       <c r="D95">
-        <v>8.8000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E95">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G95">
         <v>248</v>
@@ -3676,15 +3707,15 @@
         <v>8</v>
       </c>
       <c r="J95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>30</v>
+      <c r="A96" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B96">
         <v>231.09625</v>
@@ -3693,13 +3724,13 @@
         <v>8.4</v>
       </c>
       <c r="D96">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="E96">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G96">
         <v>248</v>
@@ -3711,15 +3742,15 @@
         <v>8</v>
       </c>
       <c r="J96" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>30</v>
+      <c r="A97" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B97">
         <v>231.09625</v>
@@ -3728,13 +3759,13 @@
         <v>8.4</v>
       </c>
       <c r="D97">
-        <v>9.1</v>
+        <v>9.4</v>
       </c>
       <c r="E97">
-        <v>9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G97">
         <v>248</v>
@@ -3746,15 +3777,15 @@
         <v>8</v>
       </c>
       <c r="J97" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>30</v>
+      <c r="A98" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B98">
         <v>231.09625</v>
@@ -3766,10 +3797,10 @@
         <v>9.4</v>
       </c>
       <c r="E98">
-        <v>9.1999999999999993</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F98" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G98">
         <v>248</v>
@@ -3781,15 +3812,15 @@
         <v>8</v>
       </c>
       <c r="J98" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K98" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>30</v>
+      <c r="A99" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B99">
         <v>231.09625</v>
@@ -3798,13 +3829,13 @@
         <v>8.4</v>
       </c>
       <c r="D99">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E99">
         <v>9.4</v>
       </c>
-      <c r="E99">
-        <v>9.3000000000000007</v>
-      </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G99">
         <v>248</v>
@@ -3816,15 +3847,15 @@
         <v>8</v>
       </c>
       <c r="J99" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K99" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>30</v>
+      <c r="A100" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B100">
         <v>231.09625</v>
@@ -3833,13 +3864,13 @@
         <v>8.4</v>
       </c>
       <c r="D100">
-        <v>9.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="E100">
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G100">
         <v>248</v>
@@ -3851,50 +3882,50 @@
         <v>8</v>
       </c>
       <c r="J100" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K100" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>30</v>
+      <c r="A101" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B101">
-        <v>231.09625</v>
+        <v>120.05</v>
       </c>
       <c r="C101">
-        <v>8.4</v>
+        <v>17.5</v>
       </c>
       <c r="D101">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="E101">
-        <v>10</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G101">
-        <v>248</v>
+        <v>340</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I101">
         <v>8</v>
       </c>
       <c r="J101" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K101" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>32</v>
+      <c r="A102" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B102">
         <v>120.05</v>
@@ -3903,13 +3934,13 @@
         <v>17.5</v>
       </c>
       <c r="D102">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="E102">
-        <v>9.3000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="F102" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G102">
         <v>340</v>
@@ -3921,15 +3952,15 @@
         <v>8</v>
       </c>
       <c r="J102" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K102" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>32</v>
       </c>
       <c r="B103">
         <v>120.05</v>
@@ -3938,13 +3969,13 @@
         <v>17.5</v>
       </c>
       <c r="D103">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="E103">
         <v>7.1</v>
       </c>
       <c r="F103" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G103">
         <v>340</v>
@@ -3956,15 +3987,15 @@
         <v>8</v>
       </c>
       <c r="J103" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>32</v>
       </c>
       <c r="B104">
         <v>120.05</v>
@@ -3973,13 +4004,13 @@
         <v>17.5</v>
       </c>
       <c r="D104">
-        <v>7.4</v>
+        <v>11</v>
       </c>
       <c r="E104">
-        <v>7.1</v>
+        <v>11.2</v>
       </c>
       <c r="F104" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G104">
         <v>340</v>
@@ -3991,15 +4022,15 @@
         <v>8</v>
       </c>
       <c r="J104" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>32</v>
       </c>
       <c r="B105">
         <v>120.05</v>
@@ -4008,13 +4039,13 @@
         <v>17.5</v>
       </c>
       <c r="D105">
-        <v>11</v>
+        <v>12.4</v>
       </c>
       <c r="E105">
-        <v>11.2</v>
+        <v>11.6</v>
       </c>
       <c r="F105" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G105">
         <v>340</v>
@@ -4026,15 +4057,15 @@
         <v>8</v>
       </c>
       <c r="J105" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K105" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>32</v>
       </c>
       <c r="B106">
         <v>120.05</v>
@@ -4043,13 +4074,13 @@
         <v>17.5</v>
       </c>
       <c r="D106">
+        <v>11.6</v>
+      </c>
+      <c r="E106">
         <v>12.4</v>
       </c>
-      <c r="E106">
-        <v>11.6</v>
-      </c>
       <c r="F106" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G106">
         <v>340</v>
@@ -4061,15 +4092,15 @@
         <v>8</v>
       </c>
       <c r="J106" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K106" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>32</v>
       </c>
       <c r="B107">
         <v>120.05</v>
@@ -4078,13 +4109,13 @@
         <v>17.5</v>
       </c>
       <c r="D107">
-        <v>11.6</v>
+        <v>10.1</v>
       </c>
       <c r="E107">
-        <v>12.4</v>
+        <v>9.9</v>
       </c>
       <c r="F107" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G107">
         <v>340</v>
@@ -4096,15 +4127,15 @@
         <v>8</v>
       </c>
       <c r="J107" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>32</v>
       </c>
       <c r="B108">
         <v>120.05</v>
@@ -4113,13 +4144,13 @@
         <v>17.5</v>
       </c>
       <c r="D108">
-        <v>10.1</v>
+        <v>11.2</v>
       </c>
       <c r="E108">
-        <v>9.9</v>
+        <v>10.9</v>
       </c>
       <c r="F108" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G108">
         <v>340</v>
@@ -4131,15 +4162,15 @@
         <v>8</v>
       </c>
       <c r="J108" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K108" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>32</v>
       </c>
       <c r="B109">
         <v>120.05</v>
@@ -4148,13 +4179,13 @@
         <v>17.5</v>
       </c>
       <c r="D109">
-        <v>11.2</v>
+        <v>12.3</v>
       </c>
       <c r="E109">
-        <v>10.9</v>
+        <v>11.6</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G109">
         <v>340</v>
@@ -4166,15 +4197,15 @@
         <v>8</v>
       </c>
       <c r="J109" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K109" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>32</v>
       </c>
       <c r="B110">
         <v>120.05</v>
@@ -4183,13 +4214,13 @@
         <v>17.5</v>
       </c>
       <c r="D110">
-        <v>12.3</v>
+        <v>8.6</v>
       </c>
       <c r="E110">
-        <v>11.6</v>
+        <v>8.6</v>
       </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G110">
         <v>340</v>
@@ -4201,45 +4232,10 @@
         <v>8</v>
       </c>
       <c r="J110" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K110" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>32</v>
-      </c>
-      <c r="B111">
-        <v>120.05</v>
-      </c>
-      <c r="C111">
-        <v>17.5</v>
-      </c>
-      <c r="D111">
-        <v>8.6</v>
-      </c>
-      <c r="E111">
-        <v>8.6</v>
-      </c>
-      <c r="F111" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111">
-        <v>340</v>
-      </c>
-      <c r="H111">
-        <v>4</v>
-      </c>
-      <c r="I111">
-        <v>8</v>
-      </c>
-      <c r="J111" t="s">
-        <v>13</v>
-      </c>
-      <c r="K111" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>